<commit_message>
Add email sending capability.
</commit_message>
<xml_diff>
--- a/notebooks/excel_gift_example/gifts.xlsx
+++ b/notebooks/excel_gift_example/gifts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neil/lawrennd/referia/notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neil/lawrennd/referia/notebooks/excel_gift_example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E54C86-7D33-F246-8029-2A0721D7314E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB04E17-272E-E84C-93E4-634C10FD48ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7820" yWindow="6840" windowWidth="28040" windowHeight="17440" xr2:uid="{F308381A-0400-0948-B6E6-A3C21C0CA0ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>G001</t>
   </si>
@@ -112,16 +112,39 @@
   </si>
   <si>
     <t>keyname</t>
+  </si>
+  <si>
+    <t>Sender Email</t>
+  </si>
+  <si>
+    <t>jenny@gmail.com</t>
+  </si>
+  <si>
+    <t>bobg@laterlly.co.uk</t>
+  </si>
+  <si>
+    <t>jen@fal.com</t>
+  </si>
+  <si>
+    <t>ban@dom.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,13 +167,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,117 +489,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987CD79-71D3-FD4A-B58E-8FD45B7B57F2}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{1390C8E7-F54B-2943-BF47-FBAD853E831C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{6ADE66DC-CF7E-6240-8DB9-5DFC23A5013E}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{E78AFB2C-C5C6-DC49-9570-D3ABCD9BEA5F}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{FD353391-6811-0243-BAF1-4B5ECC370C89}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{63DCBCE4-DDA7-F243-9DDC-C394998BB8DD}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{8D5630F5-0A07-FA47-A39F-80D25D77F5D0}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{49D4D163-50D0-7C4C-9443-1DEEBFCD6E1D}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{2F0EDCB8-92D4-1F4F-93D2-9EDB5AD98F50}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{2DB6AAE4-A30F-724A-A08E-6DEBC15EC0A0}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{068B2E4C-780E-1E41-8AB5-5122D5CD3790}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{BFE10E80-D51E-A042-BAF4-265F730D8441}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{C4BBD4D6-9FEC-A549-B09F-8CABC08FA7EB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>